<commit_message>
Update source code create new Quote from Supplier
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DataLogin.xlsx
+++ b/src/test/resources/testdata/DataLogin.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23772" windowHeight="9108" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23772" windowHeight="9108" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bettaSup" sheetId="4" r:id="rId1"/>
@@ -56,15 +56,9 @@
     <t>admin</t>
   </si>
   <si>
-    <t>https://www.amazon.com/dp/B01NGZQ9RT/ref=sspa_dk_detail_3?pd_rd_i=B01NGZQ9RT&amp;pd_rd_w=tqLfQ&amp;content-id=amzn1.sym.c4606765-78ec-444e-9319-716ceb6c5a61&amp;pf_rd_p=c4606765-78ec-444e-9319-716ceb6c5a61&amp;pf_rd_r=VR6WSZ308MKKTMWSZB8V&amp;pd_rd_wg=jcWVt&amp;pd_rd_r=66db0460-e747-4b10-8036-6047086cc190&amp;s=jewelry&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9kZXRhaWxfdGhlbWF0aWM&amp;th=1&amp;psc=1</t>
-  </si>
-  <si>
     <t>PRODUCT</t>
   </si>
   <si>
-    <t>PAVOI 14K Gold Plated X Ring Simulated Diamond CZ Criss Cross Ring for Women</t>
-  </si>
-  <si>
     <t>PRODUCT_NAME</t>
   </si>
   <si>
@@ -99,6 +93,12 @@
   </si>
   <si>
     <t>PROPERTY_VALUE</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0DQL4WS8G/ref=sspa_dk_detail_2?pd_rd_i=B0DQL4WS8G&amp;pd_rd_w=6Wscs&amp;content-id=amzn1.sym.c4606765-78ec-444e-9319-716ceb6c5a61&amp;pf_rd_p=c4606765-78ec-444e-9319-716ceb6c5a61&amp;pf_rd_r=BGKMHBF0SB0PP06EYGPZ&amp;pd_rd_wg=aH0EH&amp;pd_rd_r=1f5c7efe-de14-41df-9675-44fb20546792&amp;s=jewelry&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9kZXRhaWxfdGhlbWF0aWM&amp;th=1&amp;psc=1</t>
+  </si>
+  <si>
+    <t>Auto_Moissanite Egagement Rings for Women</t>
   </si>
 </sst>
 </file>
@@ -122,13 +122,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF0F1111"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Inherit"/>
@@ -137,6 +130,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -170,13 +170,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -571,7 +571,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -582,24 +582,21 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="55.2">
       <c r="A2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>11</v>
+        <v>22</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" display="https://www.amazon.com/dp/B01NGZQ9RT/ref=sspa_dk_detail_3?pd_rd_i=B01NGZQ9RT&amp;pd_rd_w=tqLfQ&amp;content-id=amzn1.sym.c4606765-78ec-444e-9319-716ceb6c5a61&amp;pf_rd_p=c4606765-78ec-444e-9319-716ceb6c5a61&amp;pf_rd_r=VR6WSZ308MKKTMWSZB8V&amp;pd_rd_wg=jcWVt&amp;pd_rd_r=66db0460-"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -609,72 +606,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.296875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="32.796875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="33.8984375" style="7" customWidth="1"/>
-    <col min="3" max="8" width="20.19921875" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="15.296875" style="6"/>
+    <col min="1" max="1" width="32.796875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="33.8984375" style="6" customWidth="1"/>
+    <col min="3" max="8" width="20.19921875" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="15.296875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="343.2">
+      <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="B2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="343.2">
-      <c r="A2" s="8" t="s">
+      <c r="C2" s="6">
+        <v>100</v>
+      </c>
+      <c r="D2" s="6">
+        <v>110</v>
+      </c>
+      <c r="E2" s="6">
+        <v>120</v>
+      </c>
+      <c r="F2" s="6">
+        <v>52</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="7">
-        <v>100</v>
-      </c>
-      <c r="D2" s="7">
-        <v>110</v>
-      </c>
-      <c r="E2" s="7">
-        <v>120</v>
-      </c>
-      <c r="F2" s="7">
-        <v>52</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="9"/>
+      <c r="A3" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update source code function active and add product to Store of BettaMax
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DataLogin.xlsx
+++ b/src/test/resources/testdata/DataLogin.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23772" windowHeight="9108" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23772" windowHeight="9108" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bettaSup" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>EMAIL</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>Auto_Moissanite Egagement Rings for Women</t>
+  </si>
+  <si>
+    <t>STORE_NAME</t>
+  </si>
+  <si>
+    <t>Hien store</t>
   </si>
 </sst>
 </file>
@@ -514,27 +520,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="26.69921875" customWidth="1"/>
     <col min="2" max="2" width="14.8984375" customWidth="1"/>
+    <col min="4" max="4" width="17.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -544,8 +554,11 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Source code function RFQ
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DataLogin.xlsx
+++ b/src/test/resources/testdata/DataLogin.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23772" windowHeight="9108" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23772" windowHeight="9108" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="bettaSup" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>EMAIL</t>
   </si>
@@ -95,23 +95,26 @@
     <t>PROPERTY_VALUE</t>
   </si>
   <si>
-    <t>https://www.amazon.com/dp/B0DQL4WS8G/ref=sspa_dk_detail_2?pd_rd_i=B0DQL4WS8G&amp;pd_rd_w=6Wscs&amp;content-id=amzn1.sym.c4606765-78ec-444e-9319-716ceb6c5a61&amp;pf_rd_p=c4606765-78ec-444e-9319-716ceb6c5a61&amp;pf_rd_r=BGKMHBF0SB0PP06EYGPZ&amp;pd_rd_wg=aH0EH&amp;pd_rd_r=1f5c7efe-de14-41df-9675-44fb20546792&amp;s=jewelry&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9kZXRhaWxfdGhlbWF0aWM&amp;th=1&amp;psc=1</t>
-  </si>
-  <si>
-    <t>Auto_Moissanite Egagement Rings for Women</t>
-  </si>
-  <si>
     <t>STORE_NAME</t>
   </si>
   <si>
     <t>Hien store</t>
+  </si>
+  <si>
+    <t>THE PEARL SOURCE</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B075FF6CW8?ref=emc_p_m_5_i_atc&amp;th=1</t>
+  </si>
+  <si>
+    <t>THE PEARL SOURCE Genuine Black Tahitian South Sea Cultured Pearl Karlee Hoop Earrings for Women</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,8 +141,13 @@
       <name val="Inherit"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="__Inter_d65c78"/>
+    </font>
+    <font>
       <sz val="14"/>
-      <color theme="1"/>
+      <color rgb="FF0F1111"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -166,16 +174,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -188,7 +193,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -522,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
@@ -541,7 +555,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -555,7 +569,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -581,16 +595,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="96.69921875" customWidth="1"/>
-    <col min="2" max="2" width="64.296875" customWidth="1"/>
+    <col min="1" max="1" width="96.69921875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="64.296875" style="8" customWidth="1"/>
+    <col min="3" max="16384" width="8.796875" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -601,12 +616,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="55.2">
-      <c r="A2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>23</v>
+    <row r="2" spans="1:2" ht="34.799999999999997">
+      <c r="A2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" s="9" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -625,66 +645,66 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.296875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="32.796875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="33.8984375" style="6" customWidth="1"/>
-    <col min="3" max="8" width="20.19921875" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="15.296875" style="5"/>
+    <col min="1" max="1" width="32.796875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="33.8984375" style="5" customWidth="1"/>
+    <col min="3" max="8" width="20.19921875" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="15.296875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="343.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>100</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>110</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>120</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>52</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="8"/>
+      <c r="A3" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>